<commit_message>
changed Airbus currency to USD;
</commit_message>
<xml_diff>
--- a/data/Boeing Aerospace Company report.xlsx
+++ b/data/Boeing Aerospace Company report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrylo_kundik/PycharmProjects/stockMarkets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D935C76-A6D7-B144-8952-FCC55ECB6982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9371BCD0-63DA-3149-B09C-AC393005343B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boeing Aerospace" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -229,6 +229,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,7 +380,7 @@
             <c:numRef>
               <c:f>'Boeing Aerospace'!$B$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>-12767</c:v>
@@ -476,7 +477,7 @@
             <c:numRef>
               <c:f>'Boeing Aerospace'!$B$5:$J$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2246</c:v>
@@ -573,7 +574,7 @@
             <c:numRef>
               <c:f>'Boeing Aerospace'!$B$6:$J$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>-10521</c:v>
@@ -634,7 +635,7 @@
             <c:numRef>
               <c:f>'Boeing Aerospace'!$B$8:$J$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>-11941</c:v>
@@ -757,7 +758,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -953,7 +954,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$9:$J$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>44672</c:v>
@@ -1050,7 +1051,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$13:$J$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50710</c:v>
@@ -1173,7 +1174,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1399,7 +1400,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$2:$J$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>65398</c:v>
@@ -1522,7 +1523,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1717,7 +1718,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$14:$J$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>-11255</c:v>
@@ -1840,7 +1841,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2066,7 +2067,7 @@
             <c:numRef>
               <c:f>'Boeing Aerospace'!$B$13:$J$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>152136</c:v>
@@ -3076,34 +3077,34 @@
             <c:numRef>
               <c:f>Airbus!$B$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-510</c:v>
+                  <c:v>-591.59999999999991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1339</c:v>
+                  <c:v>1553.2399999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5048</c:v>
+                  <c:v>5855.6799999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2665</c:v>
+                  <c:v>3091.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2258</c:v>
+                  <c:v>2619.2799999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4062</c:v>
+                  <c:v>4711.92</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3991</c:v>
+                  <c:v>4629.5599999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2570</c:v>
+                  <c:v>2981.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2131</c:v>
+                  <c:v>2471.96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3173,34 +3174,34 @@
             <c:numRef>
               <c:f>Airbus!$B$5:$J$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2831</c:v>
+                  <c:v>3283.9599999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2927</c:v>
+                  <c:v>3395.3199999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2444</c:v>
+                  <c:v>2835.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2298</c:v>
+                  <c:v>2665.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2294</c:v>
+                  <c:v>2661.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2466</c:v>
+                  <c:v>2860.56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2150</c:v>
+                  <c:v>2494</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1927</c:v>
+                  <c:v>2235.3199999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2053</c:v>
+                  <c:v>2381.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3270,34 +3271,34 @@
             <c:numRef>
               <c:f>Airbus!$B$6:$J$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2321</c:v>
+                  <c:v>2692.3599999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4266</c:v>
+                  <c:v>4948.5599999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7492</c:v>
+                  <c:v>8690.7199999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4963</c:v>
+                  <c:v>5757.08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4552</c:v>
+                  <c:v>5280.32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6528</c:v>
+                  <c:v>7572.48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6141</c:v>
+                  <c:v>7123.5599999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4497</c:v>
+                  <c:v>5216.5199999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4184</c:v>
+                  <c:v>4853.4400000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3367,34 +3368,34 @@
             <c:numRef>
               <c:f>Airbus!$B$8:$J$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-1169</c:v>
+                  <c:v>-1356.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1325</c:v>
+                  <c:v>-1537</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3011</c:v>
+                  <c:v>3492.7599999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2364</c:v>
+                  <c:v>2742.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>1160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2698</c:v>
+                  <c:v>3129.68</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2350</c:v>
+                  <c:v>2726</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1483</c:v>
+                  <c:v>1720.28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1229</c:v>
+                  <c:v>1425.6399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3490,7 +3491,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3686,34 +3687,34 @@
             <c:numRef>
               <c:f>Airbus!$B$9:$J$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>103639</c:v>
+                  <c:v>120221.23999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108419</c:v>
+                  <c:v>125766.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>105479</c:v>
+                  <c:v>122355.63999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98707</c:v>
+                  <c:v>114500.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107481</c:v>
+                  <c:v>124677.95999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99809</c:v>
+                  <c:v>115778.43999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89023</c:v>
+                  <c:v>103266.68</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79368</c:v>
+                  <c:v>92066.87999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81668</c:v>
+                  <c:v>94734.87999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3783,34 +3784,34 @@
             <c:numRef>
               <c:f>Airbus!$B$11:$J$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>110095</c:v>
+                  <c:v>127710.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114409</c:v>
+                  <c:v>132714.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115198</c:v>
+                  <c:v>133629.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109449</c:v>
+                  <c:v>126960.84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>111133</c:v>
+                  <c:v>128914.27999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105782</c:v>
+                  <c:v>122707.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96102</c:v>
+                  <c:v>111478.31999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90274</c:v>
+                  <c:v>104717.84</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>92102</c:v>
+                  <c:v>106838.31999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3906,7 +3907,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4132,34 +4133,34 @@
             <c:numRef>
               <c:f>Airbus!$B$2:$J$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>49912</c:v>
+                  <c:v>57897.919999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70478</c:v>
+                  <c:v>81754.48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63707</c:v>
+                  <c:v>73900.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59022</c:v>
+                  <c:v>68465.51999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66581</c:v>
+                  <c:v>77233.959999999992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64450</c:v>
+                  <c:v>74762</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60713</c:v>
+                  <c:v>70427.08</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57567</c:v>
+                  <c:v>66777.72</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56480</c:v>
+                  <c:v>65516.799999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4255,7 +4256,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4450,34 +4451,34 @@
             <c:numRef>
               <c:f>Airbus!$B$12:$J$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-9743</c:v>
+                  <c:v>-11301.879999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-10601</c:v>
+                  <c:v>-12297.159999999989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-7007</c:v>
+                  <c:v>-8128.1199999999917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-887</c:v>
+                  <c:v>-1028.9199999999983</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8416</c:v>
+                  <c:v>-9762.5600000000068</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-6582</c:v>
+                  <c:v>-7635.1199999999917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5679</c:v>
+                  <c:v>-6587.6399999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1594</c:v>
+                  <c:v>-1849.0399999999918</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2988</c:v>
+                  <c:v>-3466.0799999999963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4573,7 +4574,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4793,7 +4794,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$3:$J$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>8644</c:v>
@@ -4890,7 +4891,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$5:$J$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1290</c:v>
@@ -4987,7 +4988,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$6:$J$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>9934</c:v>
@@ -5084,7 +5085,7 @@
             <c:numRef>
               <c:f>'Lockheed Martin'!$B$8:$J$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#\ ##0.00;\(#\ ##0.00\)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6833</c:v>
@@ -5207,7 +5208,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.00;\(#\ ##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12675,7 +12676,7 @@
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16149,11 +16150,11 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16161,7 +16162,7 @@
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -16214,31 +16215,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>49912</v>
+        <v>57897.919999999998</v>
       </c>
       <c r="C2" s="5">
-        <v>70478</v>
+        <v>81754.48</v>
       </c>
       <c r="D2" s="5">
-        <v>63707</v>
+        <v>73900.12</v>
       </c>
       <c r="E2" s="5">
-        <v>59022</v>
+        <v>68465.51999999999</v>
       </c>
       <c r="F2" s="5">
-        <v>66581</v>
+        <v>77233.959999999992</v>
       </c>
       <c r="G2" s="5">
-        <v>64450</v>
+        <v>74762</v>
       </c>
       <c r="H2" s="5">
-        <v>60713</v>
+        <v>70427.08</v>
       </c>
       <c r="I2" s="5">
-        <v>57567</v>
+        <v>66777.72</v>
       </c>
       <c r="J2" s="5">
-        <v>56480</v>
+        <v>65516.799999999996</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16246,31 +16247,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>-510</v>
+        <v>-591.59999999999991</v>
       </c>
       <c r="C3" s="5">
-        <v>1339</v>
+        <v>1553.2399999999998</v>
       </c>
       <c r="D3" s="5">
-        <v>5048</v>
+        <v>5855.6799999999994</v>
       </c>
       <c r="E3" s="5">
-        <v>2665</v>
+        <v>3091.3999999999996</v>
       </c>
       <c r="F3" s="5">
-        <v>2258</v>
+        <v>2619.2799999999997</v>
       </c>
       <c r="G3" s="5">
-        <v>4062</v>
+        <v>4711.92</v>
       </c>
       <c r="H3" s="5">
-        <v>3991</v>
+        <v>4629.5599999999995</v>
       </c>
       <c r="I3" s="5">
-        <v>2570</v>
+        <v>2981.2</v>
       </c>
       <c r="J3" s="5">
-        <v>2131</v>
+        <v>2471.96</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16279,7 +16280,7 @@
       </c>
       <c r="B4" s="6">
         <f t="shared" ref="B4:J4" si="0">B3/B2*100%</f>
-        <v>-1.0217983651226158E-2</v>
+        <v>-1.0217983651226156E-2</v>
       </c>
       <c r="C4" s="6">
         <f t="shared" si="0"/>
@@ -16287,11 +16288,11 @@
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>7.9237760371701702E-2</v>
+        <v>7.9237760371701688E-2</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" si="0"/>
-        <v>4.515265494222493E-2</v>
+        <v>4.5152654942224937E-2</v>
       </c>
       <c r="F4" s="6">
         <f t="shared" si="0"/>
@@ -16313,37 +16314,38 @@
         <f t="shared" si="0"/>
         <v>3.773016997167139E-2</v>
       </c>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>2831</v>
+        <v>3283.9599999999996</v>
       </c>
       <c r="C5" s="5">
-        <v>2927</v>
+        <v>3395.3199999999997</v>
       </c>
       <c r="D5" s="5">
-        <v>2444</v>
+        <v>2835.04</v>
       </c>
       <c r="E5" s="5">
-        <v>2298</v>
+        <v>2665.68</v>
       </c>
       <c r="F5" s="5">
-        <v>2294</v>
+        <v>2661.04</v>
       </c>
       <c r="G5" s="5">
-        <v>2466</v>
+        <v>2860.56</v>
       </c>
       <c r="H5" s="5">
-        <v>2150</v>
+        <v>2494</v>
       </c>
       <c r="I5" s="5">
-        <v>1927</v>
+        <v>2235.3199999999997</v>
       </c>
       <c r="J5" s="5">
-        <v>2053</v>
+        <v>2381.48</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16352,39 +16354,39 @@
       </c>
       <c r="B6" s="5">
         <f t="shared" ref="B6:J6" si="1">B3+B5</f>
-        <v>2321</v>
+        <v>2692.3599999999997</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>4266</v>
+        <v>4948.5599999999995</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="1"/>
-        <v>7492</v>
+        <v>8690.7199999999993</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>4963</v>
+        <v>5757.08</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>4552</v>
+        <v>5280.32</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>6528</v>
+        <v>7572.48</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
-        <v>6141</v>
+        <v>7123.5599999999995</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="1"/>
-        <v>4497</v>
+        <v>5216.5199999999995</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>4184</v>
+        <v>4853.4400000000005</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16393,31 +16395,31 @@
       </c>
       <c r="B7" s="6">
         <f t="shared" ref="B7:J7" si="2">B6/B2*100%</f>
-        <v>4.6501843244109636E-2</v>
+        <v>4.6501843244109629E-2</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="2"/>
-        <v>6.052952694457845E-2</v>
+        <v>6.0529526944578443E-2</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="2"/>
-        <v>0.11760089158177281</v>
+        <v>0.1176008915817728</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="2"/>
-        <v>8.4087289485276676E-2</v>
+        <v>8.4087289485276689E-2</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="2"/>
-        <v>6.8367852690707553E-2</v>
+        <v>6.8367852690707567E-2</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="2"/>
-        <v>0.10128782001551591</v>
+        <v>0.10128782001551589</v>
       </c>
       <c r="H7" s="6">
         <f t="shared" si="2"/>
-        <v>0.10114802431110306</v>
+        <v>0.10114802431110305</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="2"/>
@@ -16425,7 +16427,7 @@
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>7.4079320113314445E-2</v>
+        <v>7.4079320113314459E-2</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16433,127 +16435,127 @@
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>-1169</v>
+        <v>-1356.04</v>
       </c>
       <c r="C8" s="5">
-        <v>-1325</v>
+        <v>-1537</v>
       </c>
       <c r="D8" s="5">
-        <v>3011</v>
+        <v>3492.7599999999998</v>
       </c>
       <c r="E8" s="5">
-        <v>2364</v>
+        <v>2742.24</v>
       </c>
       <c r="F8" s="5">
-        <v>1000</v>
+        <v>1160</v>
       </c>
       <c r="G8" s="5">
-        <v>2698</v>
+        <v>3129.68</v>
       </c>
       <c r="H8" s="5">
-        <v>2350</v>
+        <v>2726</v>
       </c>
       <c r="I8" s="5">
-        <v>1483</v>
-      </c>
-      <c r="J8" s="8">
-        <v>1229</v>
+        <v>1720.28</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1425.6399999999999</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8">
-        <v>103639</v>
-      </c>
-      <c r="C9" s="8">
-        <v>108419</v>
-      </c>
-      <c r="D9" s="8">
-        <v>105479</v>
-      </c>
-      <c r="E9" s="8">
-        <v>98707</v>
-      </c>
-      <c r="F9" s="8">
-        <v>107481</v>
-      </c>
-      <c r="G9" s="8">
-        <v>99809</v>
-      </c>
-      <c r="H9" s="8">
-        <v>89023</v>
-      </c>
-      <c r="I9" s="8">
-        <v>79368</v>
-      </c>
-      <c r="J9" s="8">
-        <v>81668</v>
+      <c r="B9" s="5">
+        <v>120221.23999999999</v>
+      </c>
+      <c r="C9" s="5">
+        <v>125766.04</v>
+      </c>
+      <c r="D9" s="5">
+        <v>122355.63999999998</v>
+      </c>
+      <c r="E9" s="5">
+        <v>114500.12</v>
+      </c>
+      <c r="F9" s="5">
+        <v>124677.95999999999</v>
+      </c>
+      <c r="G9" s="5">
+        <v>115778.43999999999</v>
+      </c>
+      <c r="H9" s="5">
+        <v>103266.68</v>
+      </c>
+      <c r="I9" s="5">
+        <v>92066.87999999999</v>
+      </c>
+      <c r="J9" s="5">
+        <v>94734.87999999999</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8">
-        <v>16199</v>
-      </c>
-      <c r="C10" s="8">
-        <v>16591</v>
-      </c>
-      <c r="D10" s="8">
-        <v>16726</v>
-      </c>
-      <c r="E10" s="8">
-        <v>11629</v>
-      </c>
-      <c r="F10" s="8">
-        <v>12068</v>
-      </c>
-      <c r="G10" s="8">
-        <v>12555</v>
-      </c>
-      <c r="H10" s="8">
-        <v>12758</v>
-      </c>
-      <c r="I10" s="8">
-        <v>12500</v>
-      </c>
-      <c r="J10" s="8">
-        <v>13422</v>
+      <c r="B10" s="5">
+        <v>18790.84</v>
+      </c>
+      <c r="C10" s="5">
+        <v>19245.559999999998</v>
+      </c>
+      <c r="D10" s="5">
+        <v>19402.16</v>
+      </c>
+      <c r="E10" s="5">
+        <v>13489.64</v>
+      </c>
+      <c r="F10" s="5">
+        <v>13998.88</v>
+      </c>
+      <c r="G10" s="5">
+        <v>14563.8</v>
+      </c>
+      <c r="H10" s="5">
+        <v>14799.279999999999</v>
+      </c>
+      <c r="I10" s="5">
+        <v>14499.999999999998</v>
+      </c>
+      <c r="J10" s="5">
+        <v>15569.519999999999</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8">
-        <v>110095</v>
-      </c>
-      <c r="C11" s="8">
-        <v>114409</v>
-      </c>
-      <c r="D11" s="8">
-        <v>115198</v>
-      </c>
-      <c r="E11" s="8">
-        <v>109449</v>
-      </c>
-      <c r="F11" s="8">
-        <v>111133</v>
-      </c>
-      <c r="G11" s="8">
-        <v>105782</v>
-      </c>
-      <c r="H11" s="8">
-        <v>96102</v>
-      </c>
-      <c r="I11" s="8">
-        <v>90274</v>
-      </c>
-      <c r="J11" s="8">
-        <v>92102</v>
+      <c r="B11" s="5">
+        <v>127710.2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>132714.44</v>
+      </c>
+      <c r="D11" s="5">
+        <v>133629.68</v>
+      </c>
+      <c r="E11" s="5">
+        <v>126960.84</v>
+      </c>
+      <c r="F11" s="5">
+        <v>128914.27999999998</v>
+      </c>
+      <c r="G11" s="5">
+        <v>122707.12</v>
+      </c>
+      <c r="H11" s="5">
+        <v>111478.31999999999</v>
+      </c>
+      <c r="I11" s="5">
+        <v>104717.84</v>
+      </c>
+      <c r="J11" s="5">
+        <v>106838.31999999999</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -16562,39 +16564,39 @@
       </c>
       <c r="B12" s="5">
         <f t="shared" ref="B12:J12" si="3">B11-B9-B10</f>
-        <v>-9743</v>
+        <v>-11301.879999999994</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="3"/>
-        <v>-10601</v>
+        <v>-12297.159999999989</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="3"/>
-        <v>-7007</v>
+        <v>-8128.1199999999917</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="3"/>
-        <v>-887</v>
+        <v>-1028.9199999999983</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="3"/>
-        <v>-8416</v>
+        <v>-9762.5600000000068</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>-6582</v>
+        <v>-7635.1199999999917</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="3"/>
-        <v>-5679</v>
+        <v>-6587.6399999999994</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="3"/>
-        <v>-1594</v>
+        <v>-1849.0399999999918</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="3"/>
-        <v>-2988</v>
+        <v>-3466.0799999999963</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -19571,7 +19573,7 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -19583,7 +19585,7 @@
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>